<commit_message>
Integrating EU data files - BPoEFUbVT, FoVObe, P, SDoVPbT, SYBSoEVP, BpTPEU, CDCF
</commit_message>
<xml_diff>
--- a/InputData/trans/SYBSoEVP/Start Year Battery Share of EV Price.xlsx
+++ b/InputData/trans/SYBSoEVP/Start Year Battery Share of EV Price.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\SYBSoEVP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murielle.gagnebin\Documents\02_ProjetsPays\01_DE\2004_EPS_Europe\eps-us-2.1.0\InputData\trans\SYBSoEVP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C817B35-5DEA-4FE4-BB05-EABD333D6C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Battery Cost Share" sheetId="3" r:id="rId2"/>
     <sheet name="SYBSoEVP" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>EV Battery Cost / kWh</t>
   </si>
@@ -35,33 +44,12 @@
     <t>Sources:</t>
   </si>
   <si>
-    <t>UBS</t>
-  </si>
-  <si>
-    <t>w/options</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
-    <t>Battery pack costs ($)</t>
-  </si>
-  <si>
-    <t>MSRP</t>
-  </si>
-  <si>
     <t>Battery share of vehicle price</t>
   </si>
   <si>
-    <t>Figure 76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q-Series: UBS Evidence Lab Electric Car Teardown - Distruption Ahead? </t>
-  </si>
-  <si>
-    <t>https://neo.ubs.com/shared/d1ZTxnvF2k/</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -72,13 +60,52 @@
   </si>
   <si>
     <t>Share of Price (dimensionless)</t>
+  </si>
+  <si>
+    <t>https://publications.jrc.ec.europa.eu/repository/bitstream/JRC113360/kjna29440enn.pdf</t>
+  </si>
+  <si>
+    <t>Average battery size in EV (Europe, in kWh)</t>
+  </si>
+  <si>
+    <t>Battery pack cost (€2017/kWh)</t>
+  </si>
+  <si>
+    <t>Battery pack costs (€2017)</t>
+  </si>
+  <si>
+    <t>Euros to Dollar 2012</t>
+  </si>
+  <si>
+    <t>€2017 to $2012, for LDVs except BEV</t>
+  </si>
+  <si>
+    <t>MSRP ($2012)</t>
+  </si>
+  <si>
+    <t>Battery pack costs ($2012)</t>
+  </si>
+  <si>
+    <t>JRC</t>
+  </si>
+  <si>
+    <t>Li-ion batteriesfor mobility and stationary storage applications - Scenarios for costs and market growth</t>
+  </si>
+  <si>
+    <t>Pages 11, 14, 66, 67</t>
+  </si>
+  <si>
+    <t>See conversion table in the InputData folder for source information.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +128,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,11 +166,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -138,10 +180,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+  <cellStyles count="3">
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -157,7 +204,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -232,6 +279,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -267,6 +331,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,14 +523,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="80.140625" customWidth="1"/>
   </cols>
@@ -469,42 +548,63 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>12</v>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>1.2179086972318509</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -513,64 +613,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>170</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <f>B3*B2</f>
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="9">
+        <f>B4*About!A16</f>
+        <v>8281.7791411765866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7">
+        <v>53641</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>12300</v>
-      </c>
-      <c r="C2">
-        <v>12300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>42635</v>
-      </c>
-      <c r="C3">
-        <v>36620</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4">
-        <f>B2/B3</f>
-        <v>0.28849536765568196</v>
-      </c>
-      <c r="C4" s="4">
-        <f>C2/C3</f>
-        <v>0.3358820316766794</v>
+      <c r="B7" s="4">
+        <f>B5/B6</f>
+        <v>0.15439270597447077</v>
       </c>
     </row>
   </sheetData>
@@ -579,24 +690,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,8 +715,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <f>AVERAGE('Battery Cost Share'!B4:C4)</f>
-        <v>0.31218869966618068</v>
+        <f>'Battery Cost Share'!B7</f>
+        <v>0.15439270597447077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to start year files, now 2019 instead of 2018; also hardcoded files are now active
</commit_message>
<xml_diff>
--- a/InputData/trans/SYBSoEVP/Start Year Battery Share of EV Price.xlsx
+++ b/InputData/trans/SYBSoEVP/Start Year Battery Share of EV Price.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murielle.gagnebin\Documents\02_ProjetsPays\01_DE\2004_EPS_Europe\eps-us-2.1.0\InputData\trans\SYBSoEVP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\trans\SYBSoEVP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C817B35-5DEA-4FE4-BB05-EABD333D6C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7EC0FD-E299-4642-8A77-1244E77DDF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Battery Cost Share" sheetId="3" r:id="rId2"/>
     <sheet name="SYBSoEVP" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>EV Battery Cost / kWh</t>
   </si>
@@ -96,6 +99,36 @@
   </si>
   <si>
     <t>See conversion table in the InputData folder for source information.</t>
+  </si>
+  <si>
+    <t>Old Numbers for 2018 Start Year:</t>
+  </si>
+  <si>
+    <t>2019 Start Year:</t>
+  </si>
+  <si>
+    <t>Battery pack cost</t>
+  </si>
+  <si>
+    <t>https://cleantechnica.com/2019/12/04/powering-the-ev-revolution-battery-packs-now-at-156-kwh-13-lower-than-2018-finds-bnef/</t>
+  </si>
+  <si>
+    <t>Bloomberg New Energy Finance (BNEF)</t>
+  </si>
+  <si>
+    <t>2019 BNEF Battery Price Survey (with Cell and Pack split)</t>
+  </si>
+  <si>
+    <t>2019 Battery Price in $/KWh</t>
+  </si>
+  <si>
+    <t>$2019 to $2012</t>
+  </si>
+  <si>
+    <t>Battery pack cost ($2019/kWh)</t>
+  </si>
+  <si>
+    <t>Battery pack costs ($2019)</t>
   </si>
 </sst>
 </file>
@@ -105,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +169,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +198,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,7 +219,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,11 +232,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,8 +253,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>191107</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40A077F8-1C5E-4EEA-8758-0F815B6CBDF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8820150" y="314325"/>
+          <a:ext cx="4629757" cy="4105275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -524,21 +623,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="80.140625" customWidth="1"/>
+    <col min="2" max="2" width="80.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -546,102 +647,146 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>156</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A25" s="8">
         <v>1.2179086972318509</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{1F0DF4DA-BD29-47F2-9CE3-B7D94B9AE9EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.40625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.76953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -649,25 +794,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>B3*B2</f>
-        <v>6800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9">
-        <f>B4*About!A16</f>
-        <v>8281.7791411765866</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <f>B4*About!A24</f>
+        <v>5603.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -675,17 +820,107 @@
         <v>53641</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="11">
         <f>B5/B6</f>
+        <v>0.10446337689453963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A11" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2010</v>
+      </c>
+      <c r="F12">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>170</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>870</v>
+      </c>
+      <c r="F13">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>B14*B13</f>
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="9">
+        <f>B15*A21</f>
+        <v>8281.7791411765866</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <v>53641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4">
+        <f>B16/B17</f>
         <v>0.15439270597447077</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>1.2179086972318509</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -697,26 +932,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <f>'Battery Cost Share'!B7</f>
-        <v>0.15439270597447077</v>
+        <v>0.10446337689453963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>